<commit_message>
Updated levels -> Added diamond and added spawn locations
</commit_message>
<xml_diff>
--- a/Data/Level/Level_1.xlsx
+++ b/Data/Level/Level_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Howest\2DAE_2023\Programming4\Projects\GameEngine\Data\Level\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E9943D9-F2E4-4449-8E7C-604DA3D364FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4539F8DD-2A23-4B47-A3E2-2DD91DA3E9AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LevelLayout0" sheetId="1" r:id="rId1"/>
@@ -891,8 +891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z10" sqref="Z10"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1067,7 +1067,7 @@
         <v>2</v>
       </c>
       <c r="AA2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB2" s="1">
         <v>0</v>
@@ -1366,7 +1366,7 @@
         <v>2</v>
       </c>
       <c r="L6" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M6" s="1">
         <v>2</v>
@@ -1683,7 +1683,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D10" s="1">
         <v>2</v>
@@ -1852,10 +1852,10 @@
         <v>0</v>
       </c>
       <c r="B12" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C12" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
@@ -1888,7 +1888,7 @@
         <v>2</v>
       </c>
       <c r="N12" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O12" s="1">
         <v>0</v>
@@ -1938,25 +1938,25 @@
         <v>0</v>
       </c>
       <c r="B13" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C13" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D13" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E13" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F13" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G13" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H13" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I13" s="1">
         <v>2</v>
@@ -1965,10 +1965,10 @@
         <v>2</v>
       </c>
       <c r="K13" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L13" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M13" s="1">
         <v>2</v>
@@ -1977,16 +1977,16 @@
         <v>2</v>
       </c>
       <c r="O13" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P13" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q13" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R13" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S13" s="1">
         <v>2</v>
@@ -1995,10 +1995,10 @@
         <v>2</v>
       </c>
       <c r="U13" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V13" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W13" s="1">
         <v>2</v>
@@ -2007,7 +2007,7 @@
         <v>2</v>
       </c>
       <c r="Y13" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z13" s="1">
         <v>2</v>
@@ -2048,7 +2048,7 @@
         <v>2</v>
       </c>
       <c r="J14" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K14" s="1">
         <v>2</v>
@@ -2116,7 +2116,7 @@
         <v>2</v>
       </c>
       <c r="D15" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E15" s="1">
         <v>2</v>
@@ -2125,10 +2125,10 @@
         <v>2</v>
       </c>
       <c r="G15" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H15" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I15" s="1">
         <v>2</v>
@@ -2137,10 +2137,10 @@
         <v>2</v>
       </c>
       <c r="K15" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L15" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M15" s="1">
         <v>2</v>
@@ -2149,10 +2149,10 @@
         <v>2</v>
       </c>
       <c r="O15" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P15" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q15" s="1">
         <v>2</v>
@@ -2161,16 +2161,16 @@
         <v>2</v>
       </c>
       <c r="S15" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T15" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U15" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V15" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W15" s="1">
         <v>2</v>
@@ -2179,7 +2179,7 @@
         <v>2</v>
       </c>
       <c r="Y15" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z15" s="1">
         <v>2</v>
@@ -2268,10 +2268,10 @@
         <v>0</v>
       </c>
       <c r="Z16" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA16" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB16" s="1">
         <v>0</v>
@@ -2354,10 +2354,10 @@
         <v>0</v>
       </c>
       <c r="Z17" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA17" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB17" s="1">
         <v>0</v>
@@ -2425,7 +2425,7 @@
         <v>2</v>
       </c>
       <c r="U18" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="V18" s="1">
         <v>2</v>
@@ -2849,7 +2849,7 @@
         <v>2</v>
       </c>
       <c r="S23" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T23" s="1">
         <v>2</v>
@@ -2893,10 +2893,10 @@
         <v>0</v>
       </c>
       <c r="E24" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F24" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G24" s="1">
         <v>0</v>
@@ -2979,10 +2979,10 @@
         <v>0</v>
       </c>
       <c r="E25" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F25" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G25" s="1">
         <v>0</v>
@@ -3059,7 +3059,7 @@
         <v>2</v>
       </c>
       <c r="C26" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D26" s="1">
         <v>2</v>

</xml_diff>